<commit_message>
2.1.2: Support class annotation and import list.
</commit_message>
<xml_diff>
--- a/meta/constants/BlancoConstantsSample.xlsx
+++ b/meta/constants/BlancoConstantsSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoConstants/meta/constants/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCBD4DF-F993-1C46-B814-DFBE3E41C463}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42F0F04-FDA6-C64C-B571-C128D99FD002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>パッケージ</t>
   </si>
@@ -250,13 +250,43 @@
       <t xml:space="preserve">セイスウチ </t>
     </rPh>
     <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>アノテーション</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>@Introspected</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>No.</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>インポートクラス名</t>
+    <rPh sb="8" eb="9">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>定数定義・インポート</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">テイスウ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>io.micronaut.core.annotation.Introspected</t>
+    <phoneticPr fontId="5"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -286,8 +316,21 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="ＭＳ ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,8 +361,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -631,11 +680,148 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -745,6 +931,39 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1092,10 +1311,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1180,28 +1399,30 @@
       <c r="E9" s="13"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="13"/>
+      <c r="A10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10"/>
       <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" s="14"/>
-      <c r="C11" s="20"/>
+      <c r="C11" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="20"/>
@@ -1209,249 +1430,334 @@
       <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
+      <c r="A13" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="19" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="6"/>
-      <c r="G17"/>
-      <c r="H17"/>
-    </row>
-    <row r="18" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A18" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="44" t="s">
+      <c r="B16" s="6"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="23"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+    </row>
+    <row r="18" spans="1:10" s="51" customFormat="1">
+      <c r="A18" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="50"/>
+    </row>
+    <row r="19" spans="1:10" s="51" customFormat="1">
+      <c r="A19" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="55"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
+    </row>
+    <row r="20" spans="1:10" s="51" customFormat="1">
+      <c r="A20" s="57">
         <v>1</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="G18"/>
-      <c r="H18"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="45"/>
-      <c r="B19" s="45"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="15"/>
-      <c r="G19"/>
-      <c r="H19"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="41">
-        <v>1</v>
-      </c>
-      <c r="B20" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="F20" s="33"/>
-      <c r="G20"/>
+      <c r="B20" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="60"/>
       <c r="H20"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="41">
-        <v>2</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="31">
-        <v>100</v>
-      </c>
-      <c r="E21" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="35"/>
-      <c r="G21"/>
+      <c r="I20"/>
+      <c r="J20"/>
+    </row>
+    <row r="21" spans="1:10" s="51" customFormat="1">
+      <c r="A21" s="57"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="60"/>
       <c r="H21"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="41"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="35"/>
-      <c r="G22"/>
+      <c r="I21"/>
+      <c r="J21"/>
+    </row>
+    <row r="22" spans="1:10" s="51" customFormat="1">
+      <c r="A22" s="63"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="60"/>
       <c r="H22"/>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="41"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="35"/>
+      <c r="I22"/>
+      <c r="J22"/>
+    </row>
+    <row r="23" spans="1:10" s="51" customFormat="1">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
       <c r="G23"/>
       <c r="H23"/>
     </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="41"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="35"/>
+    <row r="24" spans="1:10">
+      <c r="A24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="6"/>
       <c r="G24"/>
       <c r="H24"/>
     </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="41"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="35"/>
+    <row r="25" spans="1:10" ht="13.5" customHeight="1">
+      <c r="A25" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="17"/>
       <c r="G25"/>
       <c r="H25"/>
     </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="41"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="35"/>
+    <row r="26" spans="1:10">
+      <c r="A26" s="45"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="15"/>
       <c r="G26"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="41"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="35"/>
+    <row r="27" spans="1:10">
+      <c r="A27" s="41">
+        <v>1</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="33"/>
       <c r="G27"/>
       <c r="H27"/>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="42"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="37"/>
+    <row r="28" spans="1:10">
+      <c r="A28" s="41">
+        <v>2</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="31">
+        <v>100</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="35"/>
       <c r="G28"/>
       <c r="H28"/>
     </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="42"/>
+    <row r="29" spans="1:10">
+      <c r="A29" s="41"/>
       <c r="B29" s="30"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="37"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="35"/>
       <c r="G29"/>
       <c r="H29"/>
     </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="42"/>
+    <row r="30" spans="1:10">
+      <c r="A30" s="41"/>
       <c r="B30" s="30"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="37"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="35"/>
       <c r="G30"/>
       <c r="H30"/>
     </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="43"/>
-      <c r="B31" s="38"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="40"/>
+    <row r="31" spans="1:10">
+      <c r="A31" s="41"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="35"/>
       <c r="G31"/>
       <c r="H31"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:10">
+      <c r="A32" s="41"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="35"/>
       <c r="G32"/>
       <c r="H32"/>
     </row>
-    <row r="33" spans="7:8">
+    <row r="33" spans="1:8">
+      <c r="A33" s="41"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="35"/>
       <c r="G33"/>
       <c r="H33"/>
     </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="41"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="35"/>
+      <c r="G34"/>
+      <c r="H34"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="42"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="37"/>
+      <c r="G35"/>
+      <c r="H35"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="42"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="37"/>
+      <c r="G36"/>
+      <c r="H36"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="42"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="43"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="40"/>
+      <c r="G38"/>
+      <c r="H38"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="G39"/>
+      <c r="H39"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="G40"/>
+      <c r="H40"/>
+    </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D47" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D54" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>adjustConstValue</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>isAbstract</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>accessScope</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>